<commit_message>
Changes made to plot.
</commit_message>
<xml_diff>
--- a/data/data_tidy_sheeted.xlsx
+++ b/data/data_tidy_sheeted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobpollard/Desktop/Uni/1.2/BABS-2 /Report and figure/Y3948024/figure_and_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50D62D5-255C-8F4C-BDBF-D1F60A581C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30F5BC6-41BA-2843-B14C-A27CC57E56D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="840" yWindow="500" windowWidth="28480" windowHeight="15980" xr2:uid="{26FD02F4-9F24-964C-86CA-9B5543A0AD61}"/>
+    <workbookView xWindow="320" yWindow="500" windowWidth="28480" windowHeight="15980" activeTab="2" xr2:uid="{26FD02F4-9F24-964C-86CA-9B5543A0AD61}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{765CE9EC-89BD-2547-BCD5-CBAAF0F48FDB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11:I18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,7 +460,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5950000</v>
+        <v>297500</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -468,7 +468,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5250000</v>
+        <v>262500</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -476,7 +476,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>13650000</v>
+        <v>682500</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -484,7 +484,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>24000000</v>
+        <v>1200000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -492,7 +492,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>150000</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -500,7 +500,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>2600000</v>
+        <v>130000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -508,7 +508,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3450000</v>
+        <v>172500</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -516,7 +516,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>2700000</v>
+        <v>135000</v>
       </c>
     </row>
   </sheetData>
@@ -529,7 +529,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -547,7 +547,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>720000</v>
+        <v>36000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -555,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>240000</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -563,7 +563,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>180000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -571,7 +571,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1690000</v>
+        <v>84500</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -579,7 +579,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>920000</v>
+        <v>46000</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -587,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>880000</v>
+        <v>44000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -595,7 +595,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>1560000</v>
+        <v>78000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -603,7 +603,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>1200000</v>
+        <v>60000</v>
       </c>
     </row>
   </sheetData>
@@ -615,8 +615,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDBB2B8-E7A3-C840-82AC-B86D278D2CA4}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,7 +634,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>15500000</v>
+        <v>775000</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -642,7 +642,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>155000000</v>
+        <v>7750000</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -650,7 +650,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>58000000</v>
+        <v>2900000</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -658,7 +658,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2980000</v>
+        <v>149000</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -666,7 +666,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>1970000</v>
+        <v>98500</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -674,7 +674,7 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>1760000</v>
+        <v>88000</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -682,7 +682,7 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>14900000</v>
+        <v>745000</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -690,7 +690,7 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>18200000</v>
+        <v>910000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit with plots finished
</commit_message>
<xml_diff>
--- a/data/data_tidy_sheeted.xlsx
+++ b/data/data_tidy_sheeted.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobpollard/Desktop/Uni/1.2/BABS-2 /Report and figure/Y3948024/figure_and_stats/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30F5BC6-41BA-2843-B14C-A27CC57E56D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42449E1F-1C97-2D4A-9A81-F947AABFABE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="320" yWindow="500" windowWidth="28480" windowHeight="15980" activeTab="2" xr2:uid="{26FD02F4-9F24-964C-86CA-9B5543A0AD61}"/>
+    <workbookView xWindow="320" yWindow="500" windowWidth="28480" windowHeight="15980" xr2:uid="{26FD02F4-9F24-964C-86CA-9B5543A0AD61}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -441,8 +441,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{765CE9EC-89BD-2547-BCD5-CBAAF0F48FDB}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -615,7 +615,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDBB2B8-E7A3-C840-82AC-B86D278D2CA4}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>